<commit_message>
Remoção do F dos mapas e tratamento deles no código
</commit_message>
<xml_diff>
--- a/maps/Legenda.xlsx
+++ b/maps/Legenda.xlsx
@@ -153,10 +153,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>